<commit_message>
added ADC conversion, added logs
</commit_message>
<xml_diff>
--- a/doc/calculations.xlsx
+++ b/doc/calculations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UwesTechnik\invacare-g50-investigations\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A7D5B3-7703-444A-8D2F-49CB56BE5EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7BED4D-D4E1-4D90-86BF-72D5D97E57A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="1155" windowWidth="13185" windowHeight="10155" xr2:uid="{D7B498A1-AD4D-4E01-BBD3-2C96538A3792}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="17910" windowHeight="11310" activeTab="1" xr2:uid="{D7B498A1-AD4D-4E01-BBD3-2C96538A3792}"/>
   </bookViews>
   <sheets>
     <sheet name="CANbaudrate" sheetId="1" r:id="rId1"/>
+    <sheet name="Speed" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>t [µs]</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>baud rate [kBaud]</t>
+  </si>
+  <si>
+    <t>with the G40plus axle</t>
+  </si>
+  <si>
+    <t>wheel diameter [cm]</t>
+  </si>
+  <si>
+    <t>circumference [m]</t>
+  </si>
+  <si>
+    <t>turns at full speed [/s]</t>
+  </si>
+  <si>
+    <t>speed [m/s]</t>
+  </si>
+  <si>
+    <t>speed [km/h]</t>
   </si>
 </sst>
 </file>
@@ -422,7 +441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90028FF-1B4D-4C4C-9F71-AA5E06F82F0C}">
   <dimension ref="B3:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -594,4 +613,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4D1DE9-7B2C-4072-8D79-B0C18B52386A}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <f>E3/100*3.14</f>
+        <v>1.2560000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <f>E4*E6</f>
+        <v>2.5120000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <f>E8*3.6</f>
+        <v>9.0432000000000023</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>